<commit_message>
login,pdp and plp modules completed as much as possible
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/TS_Login_001_TS_Login_006_TC_Login_001_AsASuperUser_PurchaseAgent_GeneralUser.xlsx
+++ b/resources/ExcelsheetData/TS_Login_001_TS_Login_006_TC_Login_001_AsASuperUser_PurchaseAgent_GeneralUser.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Hemanth\UnilogProjects\Etna\resources\ExcelsheetData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Hemanth\UnilogProjects\etna\resources\ExcelsheetData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -66,34 +66,34 @@
     <t>Expected</t>
   </si>
   <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
     <t>webuser@unilogcorp.com</t>
   </si>
   <si>
+    <t>123456789</t>
+  </si>
+  <si>
     <t>newpurchaseagent@unilogcorp.com</t>
   </si>
   <si>
+    <t>generaluser2@unilogcorp.com</t>
+  </si>
+  <si>
     <t>Super User User</t>
   </si>
   <si>
-    <t>generaluser@unilogcorp.com</t>
-  </si>
-  <si>
-    <t>001</t>
-  </si>
-  <si>
-    <t>002</t>
-  </si>
-  <si>
-    <t>003</t>
-  </si>
-  <si>
-    <t>123456789</t>
-  </si>
-  <si>
     <t>Test Agent Test</t>
   </si>
   <si>
-    <t>Testing Last Name</t>
+    <t>General User Test User</t>
   </si>
 </sst>
 </file>
@@ -184,7 +184,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -194,6 +194,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -483,7 +484,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,27 +510,27 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>11</v>
+      <c r="C3" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>12</v>
@@ -537,13 +538,13 @@
     </row>
     <row r="4" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>11</v>
+      <c r="C4" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>13</v>
@@ -552,10 +553,8 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>